<commit_message>
Added user input, did test cases
</commit_message>
<xml_diff>
--- a/documentation/Tests.xlsx
+++ b/documentation/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\NCAA-Bracket-Predictor\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EF52BC1-E965-4309-A167-C4671F0C478C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DCABE5-DB31-44A2-B215-C78965F56497}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{9DF9FD2C-CE41-44D9-B248-E86D16A5E2AD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Test</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Added user input for indicator</t>
+  </si>
+  <si>
+    <t>Works with indicator, shows percentage and games won</t>
+  </si>
+  <si>
+    <t>Ran with inputed indicator and showed results</t>
+  </si>
+  <si>
+    <t>Works with multiple indicators</t>
   </si>
 </sst>
 </file>
@@ -93,9 +105,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -414,7 +427,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,7 +455,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>